<commit_message>
agregando verificación de precio
</commit_message>
<xml_diff>
--- a/temp/ReporteEstadoProductos.xlsx
+++ b/temp/ReporteEstadoProductos.xlsx
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="C5" s="9" t="n">
-        <v>45231.72072514542</v>
+        <v>45244.69876300471</v>
       </c>
       <c r="D5" s="5" t="n"/>
     </row>
@@ -570,46 +570,8 @@
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>PRODUCTOS INACTIVOS VENDIDOS</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>103138</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>AMORSUAVIZANTEARRULL</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>PRODUCTOS INACTIVOS VENDIDOS</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>107463</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>SUAVEPHESENCIASELEGA</t>
-        </is>
-      </c>
-    </row>
+    <row r="10"/>
+    <row r="11"/>
     <row r="12"/>
     <row r="13"/>
     <row r="14"/>

</xml_diff>